<commit_message>
4th Class finished (End) - First time i tried Data Science Stuff
</commit_message>
<xml_diff>
--- a/courses/intensivao-lira/data/Produtos_Novo.xlsx
+++ b/courses/intensivao-lira/data/Produtos_Novo.xlsx
@@ -67,25 +67,25 @@
     <t>Ouro</t>
   </si>
   <si>
-    <t>5219.65</t>
-  </si>
-  <si>
-    <t>27586.24</t>
-  </si>
-  <si>
-    <t>4697.68</t>
-  </si>
-  <si>
-    <t>4170.54</t>
-  </si>
-  <si>
-    <t>18390.83</t>
-  </si>
-  <si>
-    <t>2507.96</t>
-  </si>
-  <si>
-    <t>5882.40</t>
+    <t>7355.39</t>
+  </si>
+  <si>
+    <t>55493.21</t>
+  </si>
+  <si>
+    <t>8038.38</t>
+  </si>
+  <si>
+    <t>7136.37</t>
+  </si>
+  <si>
+    <t>35145.70</t>
+  </si>
+  <si>
+    <t>5048.79</t>
+  </si>
+  <si>
+    <t>6818.58</t>
   </si>
 </sst>
 </file>
@@ -483,16 +483,16 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>5.2197</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
+        <v>5.2539</v>
+      </c>
+      <c r="E2">
+        <v>5253.847461</v>
       </c>
       <c r="F2">
         <v>1.4</v>
       </c>
-      <c r="G2">
-        <v>6999.929999999999</v>
+      <c r="G2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -506,16 +506,16 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>6.130276665</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
+        <v>6.165912218000001</v>
+      </c>
+      <c r="E3">
+        <v>27746.604981</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>54000</v>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -529,16 +529,16 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5.2197</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
+        <v>5.2539</v>
+      </c>
+      <c r="E4">
+        <v>4728.457461</v>
       </c>
       <c r="F4">
         <v>1.7</v>
       </c>
-      <c r="G4">
-        <v>7649.914999999999</v>
+      <c r="G4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -552,16 +552,16 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>5.2197</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
+        <v>5.2539</v>
+      </c>
+      <c r="E5">
+        <v>4197.8661</v>
       </c>
       <c r="F5">
         <v>1.7</v>
       </c>
-      <c r="G5">
-        <v>6791.5</v>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -575,16 +575,16 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>6.130276665</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
+        <v>6.165912218000001</v>
+      </c>
+      <c r="E6">
+        <v>18497.736654</v>
       </c>
       <c r="F6">
         <v>1.9</v>
       </c>
-      <c r="G6">
-        <v>34200</v>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -598,16 +598,16 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>5.2197</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
+        <v>5.2539</v>
+      </c>
+      <c r="E7">
+        <v>2524.393872</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7">
-        <v>4804.8</v>
+      <c r="G7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -621,16 +621,16 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>294.12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
+        <v>296.46</v>
+      </c>
+      <c r="E8">
+        <v>5929.2</v>
       </c>
       <c r="F8">
         <v>1.15</v>
       </c>
-      <c r="G8">
-        <v>8049.999999999999</v>
+      <c r="G8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>